<commit_message>
1. new UI test
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F697F71C-F5C8-4802-A8BD-DD1B7444902F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="robot" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>未注册</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,13 +76,17 @@
   </si>
   <si>
     <t>新增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -145,7 +150,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -167,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -242,6 +246,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -277,6 +298,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -468,12 +506,10 @@
     <col min="5" max="5" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="18.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -496,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -519,8 +555,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -533,7 +569,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
@@ -542,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -564,389 +600,6 @@
       <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -956,7 +609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>